<commit_message>
correct area within buffer
</commit_message>
<xml_diff>
--- a/results/100iterations_Oct16_final.xlsx
+++ b/results/100iterations_Oct16_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wyang80\Desktop\CONN_MEASURE\data\CA\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B6E980D-5C10-42C4-901A-2162497165EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5097358C-B155-485E-B998-5906A1300EB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="100iterations_Oct16_final" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1243,10 +1243,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1350,7 +1352,7 @@
         <v>21.131699999999999</v>
       </c>
       <c r="E2">
-        <v>1539.1172590966901</v>
+        <v>277820502.38529497</v>
       </c>
       <c r="F2">
         <v>105779051.56028301</v>
@@ -1439,7 +1441,7 @@
         <v>21.4925</v>
       </c>
       <c r="E3">
-        <v>1534.81867128352</v>
+        <v>273494554.09821701</v>
       </c>
       <c r="F3">
         <v>107363855.783609</v>
@@ -1528,7 +1530,7 @@
         <v>13.7395</v>
       </c>
       <c r="E4">
-        <v>1682.63673865283</v>
+        <v>230965278.75506699</v>
       </c>
       <c r="F4">
         <v>75081305.829413995</v>
@@ -1617,7 +1619,7 @@
         <v>18.0504</v>
       </c>
       <c r="E5">
-        <v>1682.22586023997</v>
+        <v>249201930.87371299</v>
       </c>
       <c r="F5">
         <v>93237614.644358993</v>
@@ -1706,7 +1708,7 @@
         <v>21.591999999999999</v>
       </c>
       <c r="E6">
-        <v>1527.0855365902701</v>
+        <v>272865554.88393003</v>
       </c>
       <c r="F6">
         <v>108085427.325369</v>
@@ -1795,7 +1797,7 @@
         <v>22.0504</v>
       </c>
       <c r="E7">
-        <v>1631.0146475859101</v>
+        <v>268613314.09772801</v>
       </c>
       <c r="F7">
         <v>109449380.271809</v>
@@ -1884,7 +1886,7 @@
         <v>16.9877</v>
       </c>
       <c r="E8">
-        <v>1528.5165282082</v>
+        <v>249618173.0447</v>
       </c>
       <c r="F8">
         <v>88393608.384012297</v>
@@ -1973,7 +1975,7 @@
         <v>21.046800000000001</v>
       </c>
       <c r="E9">
-        <v>1606.9550878770399</v>
+        <v>267337499.38055599</v>
       </c>
       <c r="F9">
         <v>105229910.43806501</v>
@@ -2062,7 +2064,7 @@
         <v>21.246200000000002</v>
       </c>
       <c r="E10">
-        <v>1491.0368883225501</v>
+        <v>266119167.55680701</v>
       </c>
       <c r="F10">
         <v>106342810.22628599</v>
@@ -2151,7 +2153,7 @@
         <v>21.6965</v>
       </c>
       <c r="E11">
-        <v>1490.78341842703</v>
+        <v>271903710.572963</v>
       </c>
       <c r="F11">
         <v>108505668.34565701</v>
@@ -2240,7 +2242,7 @@
         <v>14.488</v>
       </c>
       <c r="E12">
-        <v>1559.5779178730299</v>
+        <v>244809224.61243099</v>
       </c>
       <c r="F12">
         <v>78207163.560342193</v>
@@ -2329,7 +2331,7 @@
         <v>21.7502</v>
       </c>
       <c r="E13">
-        <v>1617.9357409916699</v>
+        <v>274993205.52189898</v>
       </c>
       <c r="F13">
         <v>108148980.29946899</v>
@@ -2418,7 +2420,7 @@
         <v>17.228300000000001</v>
       </c>
       <c r="E14">
-        <v>1577.4168318751399</v>
+        <v>250943925.509101</v>
       </c>
       <c r="F14">
         <v>89182412.924421802</v>
@@ -2507,7 +2509,7 @@
         <v>21.3645</v>
       </c>
       <c r="E15">
-        <v>1532.17649358364</v>
+        <v>275109655.52770698</v>
       </c>
       <c r="F15">
         <v>107390003.797359</v>
@@ -2596,7 +2598,7 @@
         <v>20.887599999999999</v>
       </c>
       <c r="E16">
-        <v>1539.83603638967</v>
+        <v>270722510.95501202</v>
       </c>
       <c r="F16">
         <v>105094808.725839</v>
@@ -2685,7 +2687,7 @@
         <v>21.2652</v>
       </c>
       <c r="E17">
-        <v>1597.0040563651401</v>
+        <v>264884210.35786599</v>
       </c>
       <c r="F17">
         <v>105943828.73404101</v>
@@ -2774,7 +2776,7 @@
         <v>21.800899999999999</v>
       </c>
       <c r="E18">
-        <v>1483.74324100121</v>
+        <v>277772517.02549201</v>
       </c>
       <c r="F18">
         <v>108565070.460565</v>
@@ -2863,7 +2865,7 @@
         <v>17.0731</v>
       </c>
       <c r="E19">
-        <v>1619.4104626552</v>
+        <v>256238204.68355501</v>
       </c>
       <c r="F19">
         <v>89064696.396137193</v>
@@ -2952,7 +2954,7 @@
         <v>20.904599999999999</v>
       </c>
       <c r="E20">
-        <v>1565.1762053150701</v>
+        <v>272643535.37198001</v>
       </c>
       <c r="F20">
         <v>105252553.56979901</v>
@@ -3041,7 +3043,7 @@
         <v>21.434200000000001</v>
       </c>
       <c r="E21">
-        <v>1596.7666297824501</v>
+        <v>275980406.80915898</v>
       </c>
       <c r="F21">
         <v>107758807.217187</v>
@@ -3130,7 +3132,7 @@
         <v>21.2912</v>
       </c>
       <c r="E22">
-        <v>1522.2364487095799</v>
+        <v>283191531.606031</v>
       </c>
       <c r="F22">
         <v>107292651.357006</v>
@@ -3219,7 +3221,7 @@
         <v>21.6875</v>
       </c>
       <c r="E23">
-        <v>1532.8415200398799</v>
+        <v>270948770.57283902</v>
       </c>
       <c r="F23">
         <v>108659139.251983</v>
@@ -3308,7 +3310,7 @@
         <v>14.6776</v>
       </c>
       <c r="E24">
-        <v>1662.8133391021599</v>
+        <v>225019868.41346499</v>
       </c>
       <c r="F24">
         <v>77907878.386171699</v>
@@ -3397,7 +3399,7 @@
         <v>22.105399999999999</v>
       </c>
       <c r="E25">
-        <v>1573.67679588896</v>
+        <v>284005273.65626299</v>
       </c>
       <c r="F25">
         <v>110902359.82244299</v>
@@ -3486,7 +3488,7 @@
         <v>21.944199999999999</v>
       </c>
       <c r="E26">
-        <v>1504.0404176373399</v>
+        <v>267437123.77355</v>
       </c>
       <c r="F26">
         <v>109170053.59599499</v>
@@ -3575,7 +3577,7 @@
         <v>18.791399999999999</v>
       </c>
       <c r="E27">
-        <v>1529.67182258194</v>
+        <v>266387678.25963399</v>
       </c>
       <c r="F27">
         <v>96264767.931344301</v>
@@ -3664,7 +3666,7 @@
         <v>20.13</v>
       </c>
       <c r="E28">
-        <v>1564.33622142011</v>
+        <v>254134784.955841</v>
       </c>
       <c r="F28">
         <v>100573459.82068899</v>
@@ -3753,7 +3755,7 @@
         <v>21.277200000000001</v>
       </c>
       <c r="E29">
-        <v>1534.8309538277299</v>
+        <v>281138266.067334</v>
       </c>
       <c r="F29">
         <v>106649934.744137</v>
@@ -3842,7 +3844,7 @@
         <v>21.071899999999999</v>
       </c>
       <c r="E30">
-        <v>1533.7205162610901</v>
+        <v>268426749.42981699</v>
       </c>
       <c r="F30">
         <v>105688716.35931601</v>
@@ -3931,7 +3933,7 @@
         <v>18.217199999999998</v>
       </c>
       <c r="E31">
-        <v>1481.73856249592</v>
+        <v>265447383.65678701</v>
       </c>
       <c r="F31">
         <v>93860800.920149997</v>
@@ -4020,7 +4022,7 @@
         <v>21.122499999999999</v>
       </c>
       <c r="E32">
-        <v>1544.37187064669</v>
+        <v>266028460.27656299</v>
       </c>
       <c r="F32">
         <v>106103393.93494099</v>
@@ -4109,7 +4111,7 @@
         <v>18.072800000000001</v>
       </c>
       <c r="E33">
-        <v>1574.4215227275599</v>
+        <v>261509383.98961699</v>
       </c>
       <c r="F33">
         <v>92831051.328276098</v>
@@ -4198,7 +4200,7 @@
         <v>21.113800000000001</v>
       </c>
       <c r="E34">
-        <v>1562.1941228256901</v>
+        <v>271777503.94406402</v>
       </c>
       <c r="F34">
         <v>105809714.185739</v>
@@ -4287,7 +4289,7 @@
         <v>21.599299999999999</v>
       </c>
       <c r="E35">
-        <v>1584.1295692010699</v>
+        <v>272547928.83913702</v>
       </c>
       <c r="F35">
         <v>108153068.43479399</v>
@@ -4376,7 +4378,7 @@
         <v>21.7759</v>
       </c>
       <c r="E36">
-        <v>1574.2683000782499</v>
+        <v>279997203.19781899</v>
       </c>
       <c r="F36">
         <v>109563690.006046</v>
@@ -4465,7 +4467,7 @@
         <v>21.230799999999999</v>
       </c>
       <c r="E37">
-        <v>1565.1893262819599</v>
+        <v>276375031.585356</v>
       </c>
       <c r="F37">
         <v>106486697.553941</v>
@@ -4554,7 +4556,7 @@
         <v>18.194800000000001</v>
       </c>
       <c r="E38">
-        <v>1634.94425171843</v>
+        <v>257872995.62318599</v>
       </c>
       <c r="F38">
         <v>93849763.471639007</v>
@@ -4643,7 +4645,7 @@
         <v>21.3126</v>
       </c>
       <c r="E39">
-        <v>1506.4467456151001</v>
+        <v>276201215.574489</v>
       </c>
       <c r="F39">
         <v>107103512.281775</v>
@@ -4732,7 +4734,7 @@
         <v>17.4102</v>
       </c>
       <c r="E40">
-        <v>1550.35195989717</v>
+        <v>240332377.002736</v>
       </c>
       <c r="F40">
         <v>89408373.395589307</v>
@@ -4821,7 +4823,7 @@
         <v>17.4085</v>
       </c>
       <c r="E41">
-        <v>1581.2045539819301</v>
+        <v>241512615.73377499</v>
       </c>
       <c r="F41">
         <v>89313779.630366802</v>
@@ -4910,7 +4912,7 @@
         <v>21.8858</v>
       </c>
       <c r="E42">
-        <v>1573.0733555244101</v>
+        <v>280450199.341178</v>
       </c>
       <c r="F42">
         <v>108980452.31622</v>
@@ -4999,7 +5001,7 @@
         <v>21.789300000000001</v>
       </c>
       <c r="E43">
-        <v>1539.42746923909</v>
+        <v>278608198.977817</v>
       </c>
       <c r="F43">
         <v>108634698.22530399</v>
@@ -5088,7 +5090,7 @@
         <v>20.7316</v>
       </c>
       <c r="E44">
-        <v>1539.7838795007599</v>
+        <v>268640053.79614198</v>
       </c>
       <c r="F44">
         <v>103624933.417665</v>
@@ -5177,7 +5179,7 @@
         <v>18.440000000000001</v>
       </c>
       <c r="E45">
-        <v>1539.41040991258</v>
+        <v>256239805.56469801</v>
       </c>
       <c r="F45">
         <v>94654138.342883497</v>
@@ -5266,7 +5268,7 @@
         <v>21.889099999999999</v>
       </c>
       <c r="E46">
-        <v>1513.24318531329</v>
+        <v>271251155.47545302</v>
       </c>
       <c r="F46">
         <v>109512704.01131099</v>
@@ -5355,7 +5357,7 @@
         <v>17.916899999999998</v>
       </c>
       <c r="E47">
-        <v>1597.5361665032201</v>
+        <v>254063566.26418799</v>
       </c>
       <c r="F47">
         <v>92066714.827399403</v>
@@ -5444,7 +5446,7 @@
         <v>17.4619</v>
       </c>
       <c r="E48">
-        <v>1589.0706802745101</v>
+        <v>250195467.37032801</v>
       </c>
       <c r="F48">
         <v>90314804.724971801</v>
@@ -5533,7 +5535,7 @@
         <v>21.258600000000001</v>
       </c>
       <c r="E49">
-        <v>1522.22825205801</v>
+        <v>272026345.142169</v>
       </c>
       <c r="F49">
         <v>106580953.845682</v>
@@ -5622,7 +5624,7 @@
         <v>20.926100000000002</v>
       </c>
       <c r="E50">
-        <v>1557.4883643968201</v>
+        <v>266543962.58041</v>
       </c>
       <c r="F50">
         <v>104934406.682754</v>
@@ -5711,7 +5713,7 @@
         <v>21.303899999999999</v>
       </c>
       <c r="E51">
-        <v>1611.5245350575799</v>
+        <v>268865909.50539702</v>
       </c>
       <c r="F51">
         <v>106296306.81931201</v>
@@ -5800,7 +5802,7 @@
         <v>18.4696</v>
       </c>
       <c r="E52">
-        <v>1505.7653247994001</v>
+        <v>261148185.99293599</v>
       </c>
       <c r="F52">
         <v>95141672.324707896</v>
@@ -5889,7 +5891,7 @@
         <v>21.5258</v>
       </c>
       <c r="E53">
-        <v>1525.53735853276</v>
+        <v>271423781.55661201</v>
       </c>
       <c r="F53">
         <v>107437066.066438</v>
@@ -5978,7 +5980,7 @@
         <v>21.962499999999999</v>
       </c>
       <c r="E54">
-        <v>1485.8486249354601</v>
+        <v>276682501.89549601</v>
       </c>
       <c r="F54">
         <v>109474745.005242</v>
@@ -6067,7 +6069,7 @@
         <v>21.930399999999999</v>
       </c>
       <c r="E55">
-        <v>1602.0931096463901</v>
+        <v>269446570.54705298</v>
       </c>
       <c r="F55">
         <v>108961606.16489001</v>
@@ -6156,7 +6158,7 @@
         <v>22.012599999999999</v>
       </c>
       <c r="E56">
-        <v>1483.2972058907001</v>
+        <v>278358563.54608101</v>
       </c>
       <c r="F56">
         <v>109723138.397615</v>
@@ -6245,7 +6247,7 @@
         <v>21.866900000000001</v>
       </c>
       <c r="E57">
-        <v>1548.12652433419</v>
+        <v>272667927.83013999</v>
       </c>
       <c r="F57">
         <v>108677301.59405901</v>
@@ -6334,7 +6336,7 @@
         <v>17.706499999999998</v>
       </c>
       <c r="E58">
-        <v>1618.6441945803399</v>
+        <v>252194676.64370999</v>
       </c>
       <c r="F58">
         <v>91204043.056706205</v>
@@ -6423,7 +6425,7 @@
         <v>21.641400000000001</v>
       </c>
       <c r="E59">
-        <v>1544.5143264098699</v>
+        <v>273484936.44867301</v>
       </c>
       <c r="F59">
         <v>107714807.681044</v>
@@ -6512,7 +6514,7 @@
         <v>21.758500000000002</v>
       </c>
       <c r="E60">
-        <v>1603.1483943859</v>
+        <v>272491224.92383498</v>
       </c>
       <c r="F60">
         <v>108473527.89282399</v>
@@ -6601,7 +6603,7 @@
         <v>21.807700000000001</v>
       </c>
       <c r="E61">
-        <v>1567.9424087436701</v>
+        <v>280818715.51264399</v>
       </c>
       <c r="F61">
         <v>109249685.245535</v>
@@ -6690,7 +6692,7 @@
         <v>22.248200000000001</v>
       </c>
       <c r="E62">
-        <v>1562.8045360009501</v>
+        <v>283814453.46674502</v>
       </c>
       <c r="F62">
         <v>111269567.344881</v>
@@ -6779,7 +6781,7 @@
         <v>18.046299999999999</v>
       </c>
       <c r="E63">
-        <v>1593.27946976781</v>
+        <v>249634684.14338499</v>
       </c>
       <c r="F63">
         <v>92589228.852868006</v>
@@ -6868,7 +6870,7 @@
         <v>20.3599</v>
       </c>
       <c r="E64">
-        <v>1554.8955394720099</v>
+        <v>263721665.09923601</v>
       </c>
       <c r="F64">
         <v>102469563.318161</v>
@@ -6957,7 +6959,7 @@
         <v>21.344799999999999</v>
       </c>
       <c r="E65">
-        <v>1532.1626476941799</v>
+        <v>271030642.57695502</v>
       </c>
       <c r="F65">
         <v>106875458.244891</v>
@@ -7046,7 +7048,7 @@
         <v>18.507300000000001</v>
       </c>
       <c r="E66">
-        <v>1630.1444165862199</v>
+        <v>258780702.277354</v>
       </c>
       <c r="F66">
         <v>95443834.089104906</v>
@@ -7135,7 +7137,7 @@
         <v>21.479399999999998</v>
       </c>
       <c r="E67">
-        <v>1500.2889218094001</v>
+        <v>274910674.203426</v>
       </c>
       <c r="F67">
         <v>107381517.47868</v>
@@ -7224,7 +7226,7 @@
         <v>21.015999999999998</v>
       </c>
       <c r="E68">
-        <v>1582.4674303670299</v>
+        <v>264548065.92526501</v>
       </c>
       <c r="F68">
         <v>105332865.42245799</v>
@@ -7313,7 +7315,7 @@
         <v>17.308299999999999</v>
       </c>
       <c r="E69">
-        <v>1582.18425083958</v>
+        <v>248331729.01462299</v>
       </c>
       <c r="F69">
         <v>89810532.020572796</v>
@@ -7402,7 +7404,7 @@
         <v>21.099</v>
       </c>
       <c r="E70">
-        <v>1479.71772161488</v>
+        <v>271183268.32600302</v>
       </c>
       <c r="F70">
         <v>105695721.22353899</v>
@@ -7491,7 +7493,7 @@
         <v>21.606200000000001</v>
       </c>
       <c r="E71">
-        <v>1549.61700813364</v>
+        <v>274795567.11929202</v>
       </c>
       <c r="F71">
         <v>108135772.347656</v>
@@ -7580,7 +7582,7 @@
         <v>17.6402</v>
       </c>
       <c r="E72">
-        <v>1559.14307755051</v>
+        <v>246434199.36170101</v>
       </c>
       <c r="F72">
         <v>91390994.269981101</v>
@@ -7669,7 +7671,7 @@
         <v>21.923400000000001</v>
       </c>
       <c r="E73">
-        <v>1567.9837746354101</v>
+        <v>283696727.52098101</v>
       </c>
       <c r="F73">
         <v>109791441.96046899</v>
@@ -7758,7 +7760,7 @@
         <v>13.735799999999999</v>
       </c>
       <c r="E74">
-        <v>1675.67512034425</v>
+        <v>218850157.463824</v>
       </c>
       <c r="F74">
         <v>74424359.07626</v>
@@ -7847,7 +7849,7 @@
         <v>20.7501</v>
       </c>
       <c r="E75">
-        <v>1495.3631252003099</v>
+        <v>263765823.37341699</v>
       </c>
       <c r="F75">
         <v>103496320.18676101</v>
@@ -7936,7 +7938,7 @@
         <v>21.409700000000001</v>
       </c>
       <c r="E76">
-        <v>1608.9599147834101</v>
+        <v>278381642.49735802</v>
       </c>
       <c r="F76">
         <v>107977468.88896701</v>
@@ -8025,7 +8027,7 @@
         <v>21.729500000000002</v>
       </c>
       <c r="E77">
-        <v>1455.9268820438799</v>
+        <v>281120746.78577697</v>
       </c>
       <c r="F77">
         <v>108892969.555254</v>
@@ -8114,7 +8116,7 @@
         <v>20.933399999999999</v>
       </c>
       <c r="E78">
-        <v>1533.0413218966301</v>
+        <v>268948758.23511398</v>
       </c>
       <c r="F78">
         <v>105330273.94213399</v>
@@ -8203,7 +8205,7 @@
         <v>21.691700000000001</v>
       </c>
       <c r="E79">
-        <v>1517.1416799022199</v>
+        <v>274059780.601524</v>
       </c>
       <c r="F79">
         <v>107570335.25617801</v>
@@ -8292,7 +8294,7 @@
         <v>21.731400000000001</v>
       </c>
       <c r="E80">
-        <v>1504.4063671397801</v>
+        <v>281698385.63408399</v>
       </c>
       <c r="F80">
         <v>108498195.881089</v>
@@ -8381,7 +8383,7 @@
         <v>21.2666</v>
       </c>
       <c r="E81">
-        <v>1466.5297782589601</v>
+        <v>279704335.65184402</v>
       </c>
       <c r="F81">
         <v>107170700.6197</v>
@@ -8470,7 +8472,7 @@
         <v>20.892299999999999</v>
       </c>
       <c r="E82">
-        <v>1490.07571985186</v>
+        <v>265187394.163831</v>
       </c>
       <c r="F82">
         <v>104468797.71012101</v>
@@ -8559,7 +8561,7 @@
         <v>21.425699999999999</v>
       </c>
       <c r="E83">
-        <v>1541.3023470488199</v>
+        <v>268592925.05922699</v>
       </c>
       <c r="F83">
         <v>106470166.78763901</v>
@@ -8648,7 +8650,7 @@
         <v>20.754999999999999</v>
       </c>
       <c r="E84">
-        <v>1581.4486385723301</v>
+        <v>269456719.120242</v>
       </c>
       <c r="F84">
         <v>104581660.595006</v>
@@ -8737,7 +8739,7 @@
         <v>21.7423</v>
       </c>
       <c r="E85">
-        <v>1510.4037429417101</v>
+        <v>277713562.46017802</v>
       </c>
       <c r="F85">
         <v>108504475.87638199</v>
@@ -8826,7 +8828,7 @@
         <v>18.2942</v>
       </c>
       <c r="E86">
-        <v>1590.7026160395501</v>
+        <v>247866618.027392</v>
       </c>
       <c r="F86">
         <v>93326215.010839805</v>
@@ -8915,7 +8917,7 @@
         <v>21.4361</v>
       </c>
       <c r="E87">
-        <v>1554.38452466998</v>
+        <v>274918501.42144603</v>
       </c>
       <c r="F87">
         <v>107660095.64473</v>
@@ -9004,7 +9006,7 @@
         <v>21.3306</v>
       </c>
       <c r="E88">
-        <v>1565.6068001907299</v>
+        <v>264622819.21304601</v>
       </c>
       <c r="F88">
         <v>105918795.966655</v>
@@ -9093,7 +9095,7 @@
         <v>20.889900000000001</v>
       </c>
       <c r="E89">
-        <v>1593.36067469615</v>
+        <v>277930678.85812098</v>
       </c>
       <c r="F89">
         <v>105758961.274872</v>
@@ -9182,7 +9184,7 @@
         <v>17.944900000000001</v>
       </c>
       <c r="E90">
-        <v>1650.12768042776</v>
+        <v>248149684.21466899</v>
       </c>
       <c r="F90">
         <v>92485339.541524306</v>
@@ -9271,7 +9273,7 @@
         <v>21.766200000000001</v>
       </c>
       <c r="E91">
-        <v>1494.8966987190499</v>
+        <v>271505781.30695301</v>
       </c>
       <c r="F91">
         <v>108575688.865595</v>
@@ -9360,7 +9362,7 @@
         <v>21.214300000000001</v>
       </c>
       <c r="E92">
-        <v>1565.54697065808</v>
+        <v>280622880.61163598</v>
       </c>
       <c r="F92">
         <v>106914100.443551</v>
@@ -9449,7 +9451,7 @@
         <v>21.860900000000001</v>
       </c>
       <c r="E93">
-        <v>1437.7743509638799</v>
+        <v>278357946.89252502</v>
       </c>
       <c r="F93">
         <v>109524489.934478</v>
@@ -9538,7 +9540,7 @@
         <v>20.956</v>
       </c>
       <c r="E94">
-        <v>1493.5435206991699</v>
+        <v>260480196.44552499</v>
       </c>
       <c r="F94">
         <v>105027945.815667</v>
@@ -9627,7 +9629,7 @@
         <v>21.690100000000001</v>
       </c>
       <c r="E95">
-        <v>1609.58230846323</v>
+        <v>280543040.18167001</v>
       </c>
       <c r="F95">
         <v>108245072.12562799</v>
@@ -9716,7 +9718,7 @@
         <v>21.572800000000001</v>
       </c>
       <c r="E96">
-        <v>1532.4525588573199</v>
+        <v>284346056.07838601</v>
       </c>
       <c r="F96">
         <v>108452096.511326</v>
@@ -9805,7 +9807,7 @@
         <v>17.9312</v>
       </c>
       <c r="E97">
-        <v>1506.64004675203</v>
+        <v>244451053.14339501</v>
       </c>
       <c r="F97">
         <v>91417064.471621603</v>
@@ -9894,7 +9896,7 @@
         <v>20.783200000000001</v>
       </c>
       <c r="E98">
-        <v>1430.8586363079201</v>
+        <v>277453028.01438498</v>
       </c>
       <c r="F98">
         <v>105388255.357581</v>
@@ -9983,7 +9985,7 @@
         <v>21.578399999999998</v>
       </c>
       <c r="E99">
-        <v>1491.3544447791701</v>
+        <v>270555111.76331502</v>
       </c>
       <c r="F99">
         <v>107444524.289391</v>
@@ -10072,7 +10074,7 @@
         <v>21.618099999999998</v>
       </c>
       <c r="E100">
-        <v>1508.2833982016</v>
+        <v>267706243.112409</v>
       </c>
       <c r="F100">
         <v>108026864.495221</v>
@@ -10161,7 +10163,7 @@
         <v>17.079599999999999</v>
       </c>
       <c r="E101">
-        <v>1610.9817482626399</v>
+        <v>249198687.217141</v>
       </c>
       <c r="F101">
         <v>89328655.166377395</v>

</xml_diff>